<commit_message>
Get number of columns and rows in excel sheet
</commit_message>
<xml_diff>
--- a/src/NetCore/Saturn72.Core.Services.Tests/Resources/space-in-cols.xlsx
+++ b/src/NetCore/Saturn72.Core.Services.Tests/Resources/space-in-cols.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>B</t>
   </si>
@@ -33,7 +33,10 @@
     <t>E</t>
   </si>
   <si>
-    <t>F</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -372,15 +375,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +399,123 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>